<commit_message>
Modificacion en el documento de requerimientos, modelo MER y modelo relacional de datos
</commit_message>
<xml_diff>
--- a/Modelo relacional de datos.xlsx
+++ b/Modelo relacional de datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AdminSena/Documents/Rutas Turisticas/Rutas Git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B97EFB-CCF2-FC4D-A8CA-20F61241D13E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DA1909-B281-B047-8552-9726A819370E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25480" windowHeight="26520" activeTab="1" xr2:uid="{F8DD31EE-D1CE-E24D-9755-726946CFA497}"/>
+    <workbookView xWindow="25720" yWindow="500" windowWidth="25480" windowHeight="26520" activeTab="1" xr2:uid="{F8DD31EE-D1CE-E24D-9755-726946CFA497}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="116">
   <si>
     <t>Usuario</t>
   </si>
@@ -313,19 +313,67 @@
     <t>Fecha_reserva</t>
   </si>
   <si>
-    <t>numero_personas</t>
-  </si>
-  <si>
-    <t>acuatica</t>
-  </si>
-  <si>
-    <t>aérea</t>
-  </si>
-  <si>
-    <t>hostal</t>
-  </si>
-  <si>
-    <t>charla simbolica</t>
+    <t>camas_disponibles</t>
+  </si>
+  <si>
+    <t>podras encontrar gran variedad…</t>
+  </si>
+  <si>
+    <t>una pasadia por las diferentes …</t>
+  </si>
+  <si>
+    <t>personas_reserva</t>
+  </si>
+  <si>
+    <t>fecha_hora</t>
+  </si>
+  <si>
+    <t>10-10-2023:08:00:00</t>
+  </si>
+  <si>
+    <t>10-10-2023:08:30:00</t>
+  </si>
+  <si>
+    <t>10-10-2023:09:30:00</t>
+  </si>
+  <si>
+    <t>Tipo_taller</t>
+  </si>
+  <si>
+    <t>Almuerzos</t>
+  </si>
+  <si>
+    <t>id_almuerzo</t>
+  </si>
+  <si>
+    <t>sopa, chuleta</t>
+  </si>
+  <si>
+    <t>arroz, chicharron</t>
+  </si>
+  <si>
+    <t>12:00pm</t>
+  </si>
+  <si>
+    <t>11:30am</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>hora</t>
+  </si>
+  <si>
+    <t>apellido</t>
+  </si>
+  <si>
+    <t>sarria</t>
+  </si>
+  <si>
+    <t>lopez</t>
+  </si>
+  <si>
+    <t>precio _unitario</t>
   </si>
 </sst>
 </file>
@@ -357,7 +405,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,13 +504,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00A0FE"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFFF9AB5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -543,7 +597,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -597,6 +651,69 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -624,103 +741,28 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -732,22 +774,19 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -759,6 +798,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9AB5"/>
       <color rgb="FF00E1FF"/>
       <color rgb="FFF5AA3A"/>
       <color rgb="FFFDACFF"/>
@@ -768,7 +808,6 @@
       <color rgb="FF007DFF"/>
       <color rgb="FF00FF86"/>
       <color rgb="FF6C67FF"/>
-      <color rgb="FFFF68F5"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1105,20 +1144,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
@@ -1197,12 +1236,12 @@
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
@@ -1234,10 +1273,10 @@
         <v>45069</v>
       </c>
       <c r="F14" s="10"/>
-      <c r="M14" s="29" t="s">
+      <c r="M14" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="N14" s="30"/>
+      <c r="N14" s="23"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.2">
       <c r="M15" s="2" t="s">
@@ -1256,16 +1295,16 @@
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="23"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="44"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
@@ -1292,11 +1331,11 @@
       <c r="I22" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="M22" s="31" t="s">
+      <c r="M22" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="N22" s="32"/>
-      <c r="O22" s="33"/>
+      <c r="N22" s="25"/>
+      <c r="O22" s="26"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
@@ -1357,21 +1396,21 @@
       <c r="O28" s="1"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B29" s="44" t="s">
+      <c r="B29" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="46"/>
-      <c r="M29" s="34" t="s">
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="39"/>
+      <c r="M29" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="N29" s="35"/>
-      <c r="O29" s="36"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="29"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
@@ -1462,21 +1501,21 @@
       <c r="O37" s="1"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="26"/>
-      <c r="M38" s="37" t="s">
+      <c r="C38" s="46"/>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="47"/>
+      <c r="M38" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="N38" s="38"/>
-      <c r="O38" s="39"/>
+      <c r="N38" s="31"/>
+      <c r="O38" s="32"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
@@ -1561,11 +1600,11 @@
       <c r="O44" s="1"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="M45" s="40" t="s">
+      <c r="M45" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="N45" s="41"/>
-      <c r="O45" s="42"/>
+      <c r="N45" s="34"/>
+      <c r="O45" s="35"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.2">
       <c r="M46" s="2" t="s">
@@ -1590,15 +1629,15 @@
       </c>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B48" s="27" t="s">
+      <c r="B48" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
-      <c r="H48" s="27"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="48"/>
+      <c r="G48" s="48"/>
+      <c r="H48" s="48"/>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
@@ -1647,14 +1686,14 @@
       </c>
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="M53" s="43" t="s">
+      <c r="M53" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="N53" s="43"/>
-      <c r="O53" s="43"/>
-      <c r="P53" s="43"/>
-      <c r="Q53" s="43"/>
-      <c r="R53" s="43"/>
+      <c r="N53" s="36"/>
+      <c r="O53" s="36"/>
+      <c r="P53" s="36"/>
+      <c r="Q53" s="36"/>
+      <c r="R53" s="36"/>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.2">
       <c r="M54" s="2" t="s">
@@ -1693,14 +1732,14 @@
       <c r="S55" s="1"/>
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B57" s="28" t="s">
+      <c r="B57" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="28"/>
-      <c r="G57" s="28"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
     </row>
     <row r="58" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
@@ -1736,6 +1775,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:G57"/>
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="M22:O22"/>
@@ -1744,11 +1788,6 @@
     <mergeCell ref="M45:O45"/>
     <mergeCell ref="M53:R53"/>
     <mergeCell ref="B29:I29"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="B38:I38"/>
-    <mergeCell ref="B48:H48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5" r:id="rId1" xr:uid="{3CCEB32D-D57F-A94A-9580-F22C4758CA94}"/>
@@ -1759,10 +1798,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA610BD0-0D9A-524E-AB6D-F94BD99556AF}">
-  <dimension ref="B3:O85"/>
+  <dimension ref="B3:U85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+    <sheetView tabSelected="1" topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1774,32 +1813,36 @@
     <col min="5" max="5" width="17" style="1" customWidth="1"/>
     <col min="6" max="6" width="26.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="17.1640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="22.33203125" style="1" customWidth="1"/>
     <col min="12" max="12" width="14" style="1" customWidth="1"/>
-    <col min="13" max="13" width="21" style="1" customWidth="1"/>
-    <col min="14" max="14" width="21.1640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="21" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18.6640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="15.33203125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="14" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="19.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="21" style="1" customWidth="1"/>
+    <col min="15" max="15" width="21.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="21" style="1" customWidth="1"/>
+    <col min="17" max="17" width="18.6640625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="14" style="1" customWidth="1"/>
+    <col min="20" max="20" width="18.83203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="13.5" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="47" t="s">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B3" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1810,19 +1853,22 @@
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -1832,20 +1878,23 @@
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" s="2">
         <v>3233408379</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>123</v>
       </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>2</v>
       </c>
@@ -1855,29 +1904,32 @@
       <c r="D6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="2">
         <v>3217450988</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>1234</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B12" s="65" t="s">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B12" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="66"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-      <c r="F12" s="67"/>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="56"/>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1894,7 +1946,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <v>1</v>
       </c>
@@ -1910,12 +1962,12 @@
       <c r="F14" s="2">
         <v>1</v>
       </c>
-      <c r="M14" s="29" t="s">
+      <c r="P14" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="N14" s="30"/>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="Q14" s="23"/>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>2</v>
       </c>
@@ -1931,48 +1983,51 @@
       <c r="F15" s="2">
         <v>2</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="P15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="Q15" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="M16" s="2">
-        <v>1</v>
-      </c>
-      <c r="N16" s="2" t="s">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="P16" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="M17" s="2">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="P17" s="2">
         <v>2</v>
       </c>
-      <c r="N17" s="2" t="s">
+      <c r="Q17" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B21" s="50" t="s">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B21" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="50"/>
-      <c r="K21" s="50"/>
-      <c r="M21" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="N21" s="33"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C21" s="53"/>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="53"/>
+      <c r="M21" s="53"/>
+      <c r="O21"/>
+      <c r="P21" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q21" s="60"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
@@ -1992,26 +2047,33 @@
         <v>22</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>23</v>
+        <v>98</v>
       </c>
       <c r="I22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="K22" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J22" s="17" t="s">
+      <c r="L22" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="K22" s="53" t="s">
+      <c r="M22" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="M22" s="2" t="s">
+      <c r="N22"/>
+      <c r="P22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="N22" s="2" t="s">
+      <c r="Q22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="O22"/>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="R22"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>1</v>
       </c>
@@ -2030,27 +2092,34 @@
       <c r="G23" s="2">
         <v>10</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="2">
+        <v>5</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J23" s="7">
         <v>20000</v>
       </c>
-      <c r="I23" s="7">
-        <v>200000</v>
-      </c>
-      <c r="J23" s="2">
-        <v>1</v>
-      </c>
-      <c r="K23" s="2">
+      <c r="K23" s="7">
+        <v>100000</v>
+      </c>
+      <c r="L23" s="2">
         <v>1</v>
       </c>
       <c r="M23" s="2">
         <v>1</v>
       </c>
-      <c r="N23" s="2" t="s">
+      <c r="N23" s="10"/>
+      <c r="P23" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="O23"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="R23"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>2</v>
       </c>
@@ -2069,48 +2138,52 @@
       <c r="G24" s="2">
         <v>20</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="2">
+        <v>6</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="7">
         <v>30000</v>
       </c>
-      <c r="I24" s="7">
-        <v>600000</v>
-      </c>
-      <c r="J24" s="2">
-        <v>1</v>
-      </c>
-      <c r="K24" s="2">
-        <v>2</v>
+      <c r="K24" s="7">
+        <v>180000</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1</v>
       </c>
       <c r="M24" s="2">
         <v>2</v>
       </c>
-      <c r="N24" s="2" t="s">
+      <c r="N24" s="10"/>
+      <c r="P24" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="O24"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="O25"/>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B29" s="51" t="s">
+      <c r="R24"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="P25"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B29" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
-      <c r="K29" s="51"/>
-      <c r="M29" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="N29" s="60"/>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="52"/>
+      <c r="J29" s="52"/>
+      <c r="K29" s="52"/>
+      <c r="L29" s="52"/>
+      <c r="N29"/>
+      <c r="O29"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>29</v>
       </c>
@@ -2130,26 +2203,32 @@
         <v>22</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="I30" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K30" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J30" s="17" t="s">
+      <c r="L30" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="K30" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N30" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="O30"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="P30" s="61" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q30" s="61"/>
+      <c r="R30" s="61"/>
+      <c r="S30" s="61"/>
+      <c r="T30" s="61"/>
+      <c r="U30" s="61"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B31" s="2">
         <v>1</v>
       </c>
@@ -2168,27 +2247,43 @@
       <c r="G31" s="2">
         <v>20</v>
       </c>
-      <c r="H31" s="7">
+      <c r="H31" s="2">
+        <v>5</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J31" s="7">
         <v>30000</v>
       </c>
-      <c r="I31" s="7">
-        <v>600000</v>
-      </c>
-      <c r="J31" s="2">
-        <v>1</v>
-      </c>
-      <c r="K31" s="2">
-        <v>1</v>
-      </c>
-      <c r="M31" s="2">
-        <v>1</v>
-      </c>
-      <c r="N31" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="O31"/>
-    </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="K31" s="7">
+        <v>150000</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1</v>
+      </c>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="P31" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="S31" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="T31" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U31" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B32" s="2">
         <v>2</v>
       </c>
@@ -2208,39 +2303,78 @@
         <v>25</v>
       </c>
       <c r="H32" s="2">
+        <v>6</v>
+      </c>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2">
         <v>40000</v>
       </c>
-      <c r="I32" s="7">
-        <v>1000000</v>
-      </c>
-      <c r="J32" s="2">
+      <c r="K32" s="7">
+        <v>240000</v>
+      </c>
+      <c r="L32" s="2">
         <v>2</v>
       </c>
-      <c r="K32" s="2">
-        <v>1</v>
-      </c>
-      <c r="O32"/>
-    </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B38" s="52" t="s">
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="P32" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="R32" s="7">
+        <v>20000</v>
+      </c>
+      <c r="S32" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="T32" s="2">
+        <v>20</v>
+      </c>
+      <c r="U32" s="7">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="P33" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="R33" s="7">
+        <v>25000</v>
+      </c>
+      <c r="S33" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="T33" s="2">
+        <v>10</v>
+      </c>
+      <c r="U33" s="7">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B38" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="52"/>
-      <c r="D38" s="52"/>
-      <c r="E38" s="52"/>
-      <c r="F38" s="52"/>
-      <c r="G38" s="52"/>
-      <c r="H38" s="52"/>
-      <c r="I38" s="52"/>
-      <c r="J38" s="52"/>
-      <c r="K38" s="52"/>
-      <c r="M38" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="N38" s="58"/>
+      <c r="C38" s="51"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="51"/>
+      <c r="I38" s="51"/>
+      <c r="J38" s="51"/>
+      <c r="K38" s="51"/>
+      <c r="L38" s="51"/>
+      <c r="N38"/>
       <c r="O38"/>
-    </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P38"/>
+    </row>
+    <row r="39" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>35</v>
       </c>
@@ -2260,27 +2394,28 @@
         <v>22</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>30</v>
+        <v>98</v>
       </c>
       <c r="I39" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K39" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J39" s="17" t="s">
+      <c r="L39" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="K39" s="56" t="s">
-        <v>53</v>
-      </c>
-      <c r="L39"/>
-      <c r="M39" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N39" s="2" t="s">
-        <v>54</v>
-      </c>
+      <c r="M39"/>
+      <c r="N39"/>
       <c r="O39"/>
-    </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="P39"/>
+      <c r="Q39"/>
+      <c r="R39"/>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B40" s="2">
         <v>1</v>
       </c>
@@ -2299,27 +2434,27 @@
       <c r="G40" s="2">
         <v>4</v>
       </c>
-      <c r="H40" s="7">
+      <c r="H40" s="2">
+        <v>5</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="J40" s="7">
         <v>40000</v>
       </c>
-      <c r="I40" s="7">
+      <c r="K40" s="7">
         <v>160000</v>
       </c>
-      <c r="J40" s="2">
-        <v>1</v>
-      </c>
-      <c r="K40" s="2">
-        <v>1</v>
-      </c>
-      <c r="M40" s="2">
-        <v>1</v>
-      </c>
-      <c r="N40" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="O40"/>
-    </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="L40" s="2">
+        <v>1</v>
+      </c>
+      <c r="M40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+    </row>
+    <row r="41" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B41" s="2">
         <v>2</v>
       </c>
@@ -2338,59 +2473,54 @@
       <c r="G41" s="2">
         <v>3</v>
       </c>
-      <c r="H41" s="7">
+      <c r="H41" s="2">
+        <v>6</v>
+      </c>
+      <c r="I41" s="2"/>
+      <c r="J41" s="7">
         <v>10000</v>
       </c>
-      <c r="I41" s="7">
+      <c r="K41" s="7">
         <v>30000</v>
       </c>
-      <c r="J41" s="2">
+      <c r="L41" s="2">
         <v>2</v>
       </c>
-      <c r="K41" s="2">
-        <v>2</v>
-      </c>
-      <c r="M41" s="2">
-        <v>2</v>
-      </c>
-      <c r="N41" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="O44"/>
-    </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="O45"/>
-    </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="M46" s="59" t="s">
-        <v>49</v>
-      </c>
-      <c r="N46" s="59"/>
+      <c r="M41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+    </row>
+    <row r="44" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="P44"/>
+    </row>
+    <row r="45" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="P45"/>
+    </row>
+    <row r="46" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="N46"/>
       <c r="O46"/>
-    </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B47" s="27" t="s">
+      <c r="P46"/>
+    </row>
+    <row r="47" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B47" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="27"/>
-      <c r="J47" s="27"/>
-      <c r="K47" s="27"/>
-      <c r="M47" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="N47" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="48"/>
+      <c r="I47" s="48"/>
+      <c r="J47" s="48"/>
+      <c r="K47" s="48"/>
+      <c r="L47" s="48"/>
+      <c r="M47" s="48"/>
+      <c r="N47"/>
+      <c r="O47"/>
+      <c r="P47"/>
+    </row>
+    <row r="48" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>37</v>
       </c>
@@ -2400,35 +2530,40 @@
       <c r="D48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E48" s="64" t="s">
         <v>38</v>
       </c>
       <c r="F48" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="H48" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="I48" s="64" t="s">
+        <v>98</v>
+      </c>
+      <c r="J48" s="64" t="s">
+        <v>99</v>
+      </c>
+      <c r="K48" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I48" s="2" t="s">
+      <c r="L48" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J48" s="17" t="s">
+      <c r="M48" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="K48" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="M48" s="2">
-        <v>1</v>
-      </c>
-      <c r="N48" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="N48"/>
+      <c r="O48"/>
+      <c r="P48"/>
+      <c r="Q48"/>
+      <c r="R48"/>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B49" s="2">
         <v>1</v>
       </c>
@@ -2438,35 +2573,40 @@
       <c r="D49" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E49" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="F49" s="2">
+      <c r="F49" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G49" s="2">
         <v>2</v>
       </c>
-      <c r="G49" s="2">
+      <c r="H49" s="2">
         <v>4</v>
       </c>
-      <c r="H49" s="7">
+      <c r="I49" s="64">
+        <v>5</v>
+      </c>
+      <c r="J49" s="64" t="s">
+        <v>102</v>
+      </c>
+      <c r="K49" s="7">
         <v>45000</v>
       </c>
-      <c r="I49" s="7">
+      <c r="L49" s="7">
         <v>180000</v>
       </c>
-      <c r="J49" s="2">
-        <v>1</v>
-      </c>
-      <c r="K49" s="2">
-        <v>1</v>
-      </c>
       <c r="M49" s="2">
-        <v>2</v>
-      </c>
-      <c r="N49" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="N49"/>
+      <c r="O49"/>
+      <c r="P49"/>
+      <c r="Q49"/>
+      <c r="R49"/>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B50" s="2">
         <v>2</v>
       </c>
@@ -2476,39 +2616,45 @@
       <c r="D50" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E50" s="64">
         <v>8</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="F50" s="2">
+        <v>20</v>
+      </c>
+      <c r="G50" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G50" s="2">
+      <c r="H50" s="2">
         <v>6</v>
       </c>
-      <c r="H50" s="7">
+      <c r="I50" s="64">
+        <v>6</v>
+      </c>
+      <c r="J50" s="64"/>
+      <c r="K50" s="7">
         <v>30000</v>
       </c>
-      <c r="I50" s="7">
+      <c r="L50" s="7">
         <v>180000</v>
       </c>
-      <c r="J50" s="2">
+      <c r="M50" s="2">
         <v>2</v>
       </c>
-      <c r="K50" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B56" s="61" t="s">
+      <c r="N50"/>
+      <c r="O50"/>
+    </row>
+    <row r="56" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B56" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="C56" s="62"/>
-      <c r="D56" s="62"/>
-      <c r="E56" s="63"/>
+      <c r="C56" s="58"/>
+      <c r="D56" s="58"/>
+      <c r="E56" s="59"/>
       <c r="F56"/>
       <c r="G56"/>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="s">
         <v>41</v>
       </c>
@@ -2522,81 +2668,86 @@
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B58" s="2">
         <v>1</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D58" s="2"/>
+      <c r="D58" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="E58" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B59" s="2">
         <v>2</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D59" s="2"/>
+      <c r="D59" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="E59" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
     </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B62"/>
       <c r="C62"/>
       <c r="D62"/>
     </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B63"/>
       <c r="C63"/>
       <c r="D63"/>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B64"/>
       <c r="C64"/>
       <c r="D64"/>
     </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B65"/>
       <c r="C65"/>
       <c r="D65"/>
     </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B66"/>
       <c r="C66"/>
       <c r="D66"/>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B67" s="68" t="s">
+    <row r="67" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B67" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="C67" s="69"/>
-      <c r="D67" s="69"/>
-      <c r="E67" s="69"/>
-      <c r="F67" s="69"/>
-      <c r="G67" s="69"/>
-      <c r="H67" s="69"/>
-      <c r="I67" s="69"/>
-      <c r="J67" s="69"/>
-      <c r="K67" s="69"/>
+      <c r="C67" s="50"/>
+      <c r="D67" s="50"/>
+      <c r="E67" s="50"/>
+      <c r="F67" s="50"/>
+      <c r="G67" s="50"/>
+      <c r="H67" s="50"/>
+      <c r="I67" s="50"/>
+      <c r="J67" s="50"/>
+      <c r="K67" s="50"/>
       <c r="L67"/>
-    </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M67"/>
+    </row>
+    <row r="68" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B68" s="2" t="s">
         <v>60</v>
       </c>
@@ -2615,20 +2766,23 @@
       <c r="G68" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H68" s="64" t="s">
+      <c r="H68" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I68" s="2" t="s">
+      <c r="I68" s="62" t="s">
+        <v>105</v>
+      </c>
+      <c r="J68" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="J68" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="K68" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L68" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B69" s="2">
         <v>1</v>
       </c>
@@ -2650,67 +2804,70 @@
       <c r="H69" s="2">
         <v>1</v>
       </c>
-      <c r="I69" s="5">
+      <c r="I69" s="2">
+        <v>2</v>
+      </c>
+      <c r="J69" s="5">
         <v>45209</v>
       </c>
-      <c r="J69" s="2">
+      <c r="K69" s="2">
         <v>23</v>
       </c>
-      <c r="K69" s="2">
+      <c r="L69" s="2">
         <v>350000</v>
       </c>
     </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B70"/>
       <c r="C70"/>
       <c r="D70"/>
     </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B71"/>
       <c r="C71"/>
       <c r="D71"/>
     </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B72"/>
       <c r="C72"/>
       <c r="D72"/>
     </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
     </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
     </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76"/>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77"/>
     </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78"/>
     </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79"/>
     </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80"/>
@@ -2741,24 +2898,22 @@
       <c r="D85"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="11">
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="B21:M21"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="P30:U30"/>
     <mergeCell ref="B67:K67"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B38:K38"/>
-    <mergeCell ref="B29:K29"/>
-    <mergeCell ref="B21:K21"/>
-    <mergeCell ref="M38:N38"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="B47:K47"/>
-    <mergeCell ref="M29:N29"/>
     <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B47:M47"/>
+    <mergeCell ref="B3:I3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1" xr:uid="{75F1E996-0DAC-A046-8A72-3230C587CEA0}"/>
-    <hyperlink ref="F6" r:id="rId2" xr:uid="{4AE89AD5-6878-DF4D-8FEC-6F00EBEF9266}"/>
+    <hyperlink ref="G5" r:id="rId1" xr:uid="{75F1E996-0DAC-A046-8A72-3230C587CEA0}"/>
+    <hyperlink ref="G6" r:id="rId2" xr:uid="{4AE89AD5-6878-DF4D-8FEC-6F00EBEF9266}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modificacion del documento de especificacion de requerimientos
</commit_message>
<xml_diff>
--- a/Modelo relacional de datos.xlsx
+++ b/Modelo relacional de datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AdminSena/Documents/Rutas Turisticas/Rutas Git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B317979-BC6E-B74B-BEE8-F99F8EB00B41}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525FB65C-5D2C-904B-B15B-F2A032530999}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25720" yWindow="500" windowWidth="25480" windowHeight="26520" activeTab="1" xr2:uid="{F8DD31EE-D1CE-E24D-9755-726946CFA497}"/>
+    <workbookView xWindow="1960" yWindow="500" windowWidth="25480" windowHeight="26520" activeTab="1" xr2:uid="{F8DD31EE-D1CE-E24D-9755-726946CFA497}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -594,7 +594,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -654,6 +654,39 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -711,55 +744,28 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -771,19 +777,7 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1141,20 +1135,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="41"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="41"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="24"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
@@ -1233,12 +1227,12 @@
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
@@ -1270,10 +1264,10 @@
         <v>45069</v>
       </c>
       <c r="F14" s="10"/>
-      <c r="M14" s="22" t="s">
+      <c r="M14" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="N14" s="23"/>
+      <c r="N14" s="34"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.2">
       <c r="M15" s="2" t="s">
@@ -1292,16 +1286,16 @@
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="44"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="27"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
@@ -1328,11 +1322,11 @@
       <c r="I22" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="M22" s="24" t="s">
+      <c r="M22" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="N22" s="25"/>
-      <c r="O22" s="26"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="37"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
@@ -1393,21 +1387,21 @@
       <c r="O28" s="1"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="39"/>
-      <c r="M29" s="27" t="s">
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="50"/>
+      <c r="M29" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="N29" s="28"/>
-      <c r="O29" s="29"/>
+      <c r="N29" s="39"/>
+      <c r="O29" s="40"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
@@ -1498,21 +1492,21 @@
       <c r="O37" s="1"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B38" s="45" t="s">
+      <c r="B38" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="46"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="46"/>
-      <c r="G38" s="46"/>
-      <c r="H38" s="46"/>
-      <c r="I38" s="47"/>
-      <c r="M38" s="30" t="s">
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="30"/>
+      <c r="M38" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="N38" s="31"/>
-      <c r="O38" s="32"/>
+      <c r="N38" s="42"/>
+      <c r="O38" s="43"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
@@ -1597,11 +1591,11 @@
       <c r="O44" s="1"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="M45" s="33" t="s">
+      <c r="M45" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="N45" s="34"/>
-      <c r="O45" s="35"/>
+      <c r="N45" s="45"/>
+      <c r="O45" s="46"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.2">
       <c r="M46" s="2" t="s">
@@ -1626,15 +1620,15 @@
       </c>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B48" s="48" t="s">
+      <c r="B48" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C48" s="48"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="48"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+      <c r="H48" s="31"/>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
@@ -1683,14 +1677,14 @@
       </c>
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="M53" s="36" t="s">
+      <c r="M53" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="N53" s="36"/>
-      <c r="O53" s="36"/>
-      <c r="P53" s="36"/>
-      <c r="Q53" s="36"/>
-      <c r="R53" s="36"/>
+      <c r="N53" s="47"/>
+      <c r="O53" s="47"/>
+      <c r="P53" s="47"/>
+      <c r="Q53" s="47"/>
+      <c r="R53" s="47"/>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.2">
       <c r="M54" s="2" t="s">
@@ -1729,14 +1723,14 @@
       <c r="S55" s="1"/>
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="C57" s="21"/>
-      <c r="D57" s="21"/>
-      <c r="E57" s="21"/>
-      <c r="F57" s="21"/>
-      <c r="G57" s="21"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="32"/>
+      <c r="F57" s="32"/>
+      <c r="G57" s="32"/>
     </row>
     <row r="58" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
@@ -1772,11 +1766,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="B38:I38"/>
-    <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:G57"/>
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="M22:O22"/>
@@ -1785,6 +1774,11 @@
     <mergeCell ref="M45:O45"/>
     <mergeCell ref="M53:R53"/>
     <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="B48:H48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5" r:id="rId1" xr:uid="{3CCEB32D-D57F-A94A-9580-F22C4758CA94}"/>
@@ -1797,8 +1791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA610BD0-0D9A-524E-AB6D-F94BD99556AF}">
   <dimension ref="B3:U85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M17" workbookViewId="0">
-      <selection activeCell="Q41" sqref="Q41"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1828,16 +1822,16 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="62"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
@@ -1918,13 +1912,13 @@
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="56"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="53"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
@@ -1959,10 +1953,10 @@
       <c r="F14" s="2">
         <v>1</v>
       </c>
-      <c r="P14" s="22" t="s">
+      <c r="P14" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="Q14" s="23"/>
+      <c r="Q14" s="34"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
@@ -2004,25 +1998,25 @@
       </c>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B21" s="53" t="s">
+      <c r="B21" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="53"/>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="53"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="53"/>
-      <c r="I21" s="53"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="53"/>
-      <c r="L21" s="53"/>
-      <c r="M21" s="53"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="54"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="54"/>
+      <c r="M21" s="54"/>
       <c r="O21"/>
-      <c r="P21" s="60" t="s">
+      <c r="P21" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="Q21" s="60"/>
+      <c r="Q21" s="57"/>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
@@ -2164,19 +2158,19 @@
       <c r="P25"/>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B29" s="52" t="s">
+      <c r="B29" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="52"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="52"/>
-      <c r="K29" s="52"/>
-      <c r="L29" s="52"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="55"/>
+      <c r="L29" s="55"/>
       <c r="N29"/>
       <c r="O29"/>
     </row>
@@ -2216,14 +2210,14 @@
       </c>
       <c r="M30"/>
       <c r="N30"/>
-      <c r="P30" s="61" t="s">
+      <c r="P30" s="58" t="s">
         <v>105</v>
       </c>
-      <c r="Q30" s="61"/>
-      <c r="R30" s="61"/>
-      <c r="S30" s="61"/>
-      <c r="T30" s="61"/>
-      <c r="U30" s="61"/>
+      <c r="Q30" s="58"/>
+      <c r="R30" s="58"/>
+      <c r="S30" s="58"/>
+      <c r="T30" s="58"/>
+      <c r="U30" s="58"/>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B31" s="2">
@@ -2354,19 +2348,19 @@
       </c>
     </row>
     <row r="38" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B38" s="51" t="s">
+      <c r="B38" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="51"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="51"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="51"/>
-      <c r="H38" s="51"/>
-      <c r="I38" s="51"/>
-      <c r="J38" s="51"/>
-      <c r="K38" s="51"/>
-      <c r="L38" s="51"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="56"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="56"/>
+      <c r="J38" s="56"/>
+      <c r="K38" s="56"/>
+      <c r="L38" s="56"/>
       <c r="N38"/>
       <c r="O38"/>
       <c r="P38"/>
@@ -2499,20 +2493,20 @@
       <c r="P46"/>
     </row>
     <row r="47" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B47" s="48" t="s">
+      <c r="B47" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="48"/>
-      <c r="H47" s="48"/>
-      <c r="I47" s="48"/>
-      <c r="J47" s="48"/>
-      <c r="K47" s="48"/>
-      <c r="L47" s="48"/>
-      <c r="M47" s="48"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="31"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
+      <c r="K47" s="31"/>
+      <c r="L47" s="31"/>
+      <c r="M47" s="31"/>
       <c r="N47"/>
       <c r="O47"/>
       <c r="P47"/>
@@ -2527,7 +2521,7 @@
       <c r="D48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E48" s="64" t="s">
+      <c r="E48" s="22" t="s">
         <v>38</v>
       </c>
       <c r="F48" s="2" t="s">
@@ -2539,10 +2533,10 @@
       <c r="H48" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I48" s="64" t="s">
+      <c r="I48" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="J48" s="64" t="s">
+      <c r="J48" s="22" t="s">
         <v>99</v>
       </c>
       <c r="K48" s="2" t="s">
@@ -2570,7 +2564,7 @@
       <c r="D49" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E49" s="64" t="s">
+      <c r="E49" s="22" t="s">
         <v>72</v>
       </c>
       <c r="F49" s="2" t="s">
@@ -2582,10 +2576,10 @@
       <c r="H49" s="2">
         <v>4</v>
       </c>
-      <c r="I49" s="64">
+      <c r="I49" s="22">
         <v>5</v>
       </c>
-      <c r="J49" s="64" t="s">
+      <c r="J49" s="22" t="s">
         <v>102</v>
       </c>
       <c r="K49" s="7">
@@ -2613,7 +2607,7 @@
       <c r="D50" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E50" s="64">
+      <c r="E50" s="22">
         <v>8</v>
       </c>
       <c r="F50" s="2">
@@ -2625,10 +2619,10 @@
       <c r="H50" s="2">
         <v>6</v>
       </c>
-      <c r="I50" s="64">
+      <c r="I50" s="22">
         <v>6</v>
       </c>
-      <c r="J50" s="64"/>
+      <c r="J50" s="22"/>
       <c r="K50" s="7">
         <v>30000</v>
       </c>
@@ -2642,12 +2636,12 @@
       <c r="O50"/>
     </row>
     <row r="56" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B56" s="57" t="s">
+      <c r="B56" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="C56" s="58"/>
-      <c r="D56" s="58"/>
-      <c r="E56" s="59"/>
+      <c r="C56" s="60"/>
+      <c r="D56" s="60"/>
+      <c r="E56" s="61"/>
       <c r="F56"/>
       <c r="G56"/>
     </row>
@@ -2729,19 +2723,19 @@
       <c r="D66"/>
     </row>
     <row r="67" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B67" s="49" t="s">
+      <c r="B67" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="C67" s="50"/>
-      <c r="D67" s="50"/>
-      <c r="E67" s="50"/>
-      <c r="F67" s="50"/>
-      <c r="G67" s="50"/>
-      <c r="H67" s="50"/>
-      <c r="I67" s="50"/>
-      <c r="J67" s="50"/>
-      <c r="K67" s="50"/>
-      <c r="L67"/>
+      <c r="C67" s="47"/>
+      <c r="D67" s="47"/>
+      <c r="E67" s="47"/>
+      <c r="F67" s="47"/>
+      <c r="G67" s="47"/>
+      <c r="H67" s="47"/>
+      <c r="I67" s="47"/>
+      <c r="J67" s="47"/>
+      <c r="K67" s="47"/>
+      <c r="L67" s="47"/>
       <c r="M67"/>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.2">
@@ -2766,7 +2760,7 @@
       <c r="H68" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I68" s="62" t="s">
+      <c r="I68" s="21" t="s">
         <v>104</v>
       </c>
       <c r="J68" s="2" t="s">
@@ -2896,6 +2890,10 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B47:M47"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B67:L67"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="P14:Q14"/>
     <mergeCell ref="B21:M21"/>
@@ -2903,10 +2901,6 @@
     <mergeCell ref="B38:L38"/>
     <mergeCell ref="P21:Q21"/>
     <mergeCell ref="P30:U30"/>
-    <mergeCell ref="B67:K67"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B47:M47"/>
-    <mergeCell ref="B3:I3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{75F1E996-0DAC-A046-8A72-3230C587CEA0}"/>

</xml_diff>

<commit_message>
Modificacion modelo MER, modelo relacional de datos y Diccionario de datos
</commit_message>
<xml_diff>
--- a/Modelo relacional de datos.xlsx
+++ b/Modelo relacional de datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AdminSena/Documents/Rutas Turisticas/Rutas Git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929A0896-FCD7-804C-AA3F-C221481E9664}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A55FF30-8949-774B-A5E4-0FB0B27BA972}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="500" windowWidth="25480" windowHeight="26520" activeTab="1" xr2:uid="{F8DD31EE-D1CE-E24D-9755-726946CFA497}"/>
+    <workbookView xWindow="140" yWindow="500" windowWidth="23560" windowHeight="26520" activeTab="1" xr2:uid="{F8DD31EE-D1CE-E24D-9755-726946CFA497}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="108">
   <si>
     <t>Usuario</t>
   </si>
@@ -310,9 +310,6 @@
     <t>taller religioso</t>
   </si>
   <si>
-    <t>Fecha_reserva</t>
-  </si>
-  <si>
     <t>camas_disponibles</t>
   </si>
   <si>
@@ -322,45 +319,18 @@
     <t>una pasadia por las diferentes …</t>
   </si>
   <si>
-    <t>personas_reserva</t>
-  </si>
-  <si>
-    <t>fecha_hora</t>
-  </si>
-  <si>
-    <t>10-10-2023:08:00:00</t>
-  </si>
-  <si>
-    <t>10-10-2023:08:30:00</t>
-  </si>
-  <si>
-    <t>10-10-2023:09:30:00</t>
-  </si>
-  <si>
     <t>Tipo_taller</t>
   </si>
   <si>
     <t>id_almuerzo</t>
   </si>
   <si>
-    <t>Menu</t>
-  </si>
-  <si>
     <t>sopa, chuleta</t>
   </si>
   <si>
     <t>arroz, chicharron</t>
   </si>
   <si>
-    <t>12:00pm</t>
-  </si>
-  <si>
-    <t>11:30am</t>
-  </si>
-  <si>
-    <t>hora</t>
-  </si>
-  <si>
     <t>apellido</t>
   </si>
   <si>
@@ -371,6 +341,15 @@
   </si>
   <si>
     <t>precio _unitario</t>
+  </si>
+  <si>
+    <t>cantidad_max_personas</t>
+  </si>
+  <si>
+    <t>Almuerzo</t>
+  </si>
+  <si>
+    <t>menu</t>
   </si>
 </sst>
 </file>
@@ -402,7 +381,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -511,14 +490,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -589,12 +562,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -657,7 +650,70 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -687,61 +743,16 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -753,31 +764,28 @@
     <xf numFmtId="0" fontId="1" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1135,20 +1143,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
@@ -1227,12 +1235,12 @@
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
@@ -1264,10 +1272,10 @@
         <v>45069</v>
       </c>
       <c r="F14" s="10"/>
-      <c r="M14" s="33" t="s">
+      <c r="M14" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="N14" s="34"/>
+      <c r="N14" s="27"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.2">
       <c r="M15" s="2" t="s">
@@ -1286,16 +1294,16 @@
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="27"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="48"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
@@ -1322,11 +1330,11 @@
       <c r="I22" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="M22" s="35" t="s">
+      <c r="M22" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="N22" s="36"/>
-      <c r="O22" s="37"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="30"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
@@ -1387,21 +1395,21 @@
       <c r="O28" s="1"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
-      <c r="E29" s="49"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="50"/>
-      <c r="M29" s="38" t="s">
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="43"/>
+      <c r="M29" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="N29" s="39"/>
-      <c r="O29" s="40"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="33"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
@@ -1492,21 +1500,21 @@
       <c r="O37" s="1"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="30"/>
-      <c r="M38" s="41" t="s">
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="51"/>
+      <c r="M38" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="N38" s="42"/>
-      <c r="O38" s="43"/>
+      <c r="N38" s="35"/>
+      <c r="O38" s="36"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
@@ -1591,11 +1599,11 @@
       <c r="O44" s="1"/>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="M45" s="44" t="s">
+      <c r="M45" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="N45" s="45"/>
-      <c r="O45" s="46"/>
+      <c r="N45" s="38"/>
+      <c r="O45" s="39"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.2">
       <c r="M46" s="2" t="s">
@@ -1620,15 +1628,15 @@
       </c>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B48" s="31" t="s">
+      <c r="B48" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="C48" s="31"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="31"/>
-      <c r="G48" s="31"/>
-      <c r="H48" s="31"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="52"/>
+      <c r="F48" s="52"/>
+      <c r="G48" s="52"/>
+      <c r="H48" s="52"/>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
@@ -1677,14 +1685,14 @@
       </c>
     </row>
     <row r="53" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="M53" s="47" t="s">
+      <c r="M53" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="N53" s="47"/>
-      <c r="O53" s="47"/>
-      <c r="P53" s="47"/>
-      <c r="Q53" s="47"/>
-      <c r="R53" s="47"/>
+      <c r="N53" s="40"/>
+      <c r="O53" s="40"/>
+      <c r="P53" s="40"/>
+      <c r="Q53" s="40"/>
+      <c r="R53" s="40"/>
     </row>
     <row r="54" spans="2:19" x14ac:dyDescent="0.2">
       <c r="M54" s="2" t="s">
@@ -1723,14 +1731,14 @@
       <c r="S55" s="1"/>
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B57" s="32" t="s">
+      <c r="B57" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C57" s="32"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="32"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="32"/>
+      <c r="C57" s="25"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="25"/>
+      <c r="G57" s="25"/>
     </row>
     <row r="58" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
@@ -1766,6 +1774,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="B48:H48"/>
     <mergeCell ref="B57:G57"/>
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="M22:O22"/>
@@ -1774,11 +1787,6 @@
     <mergeCell ref="M45:O45"/>
     <mergeCell ref="M53:R53"/>
     <mergeCell ref="B29:I29"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="B38:I38"/>
-    <mergeCell ref="B48:H48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5" r:id="rId1" xr:uid="{3CCEB32D-D57F-A94A-9580-F22C4758CA94}"/>
@@ -1789,10 +1797,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA610BD0-0D9A-524E-AB6D-F94BD99556AF}">
-  <dimension ref="B3:U85"/>
+  <dimension ref="B3:S83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView tabSelected="1" topLeftCell="C47" workbookViewId="0">
+      <selection activeCell="O55" sqref="O55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1803,7 +1811,7 @@
     <col min="4" max="4" width="21.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" customWidth="1"/>
     <col min="6" max="6" width="26.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.83203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="19.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="17.1640625" style="1" customWidth="1"/>
@@ -1821,19 +1829,19 @@
     <col min="22" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B3" s="62" t="s">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B3" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1844,7 +1852,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>4</v>
@@ -1859,7 +1867,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -1870,7 +1878,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="F5" s="2">
         <v>3233408379</v>
@@ -1885,7 +1893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>2</v>
       </c>
@@ -1896,7 +1904,7 @@
         <v>81</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="F6" s="2">
         <v>3217450988</v>
@@ -1911,16 +1919,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B12" s="51" t="s">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B12" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="53"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="59"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1937,7 +1945,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <v>1</v>
       </c>
@@ -1953,12 +1961,12 @@
       <c r="F14" s="2">
         <v>1</v>
       </c>
-      <c r="P14" s="33" t="s">
+      <c r="O14" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="Q14" s="34"/>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="P14" s="23"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>2</v>
       </c>
@@ -1974,51 +1982,50 @@
       <c r="F15" s="2">
         <v>2</v>
       </c>
+      <c r="O15" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="P15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q15" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="P16" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="2" t="s">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="O16" s="2">
+        <v>1</v>
+      </c>
+      <c r="P16" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="P17" s="2">
+    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="O17" s="2">
         <v>2</v>
       </c>
-      <c r="Q17" s="2" t="s">
+      <c r="P17" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B21" s="54" t="s">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B21" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
-      <c r="M21" s="54"/>
-      <c r="O21"/>
-      <c r="P21" s="57" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q21" s="57"/>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="48"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="O21" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="P21" s="24"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
@@ -2035,36 +2042,29 @@
         <v>21</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="K22" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="L22" s="17" t="s">
+      <c r="J22" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="M22" s="19" t="s">
+      <c r="K22" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="N22"/>
+      <c r="L22"/>
+      <c r="O22" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="P22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="R22"/>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>1</v>
       </c>
@@ -2083,34 +2083,27 @@
       <c r="G23" s="2">
         <v>10</v>
       </c>
-      <c r="H23" s="2">
-        <v>5</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="J23" s="7">
+      <c r="H23" s="7">
         <v>20000</v>
       </c>
-      <c r="K23" s="7">
+      <c r="I23" s="7">
         <v>100000</v>
       </c>
-      <c r="L23" s="2">
-        <v>1</v>
-      </c>
-      <c r="M23" s="2">
-        <v>1</v>
-      </c>
-      <c r="N23" s="10"/>
-      <c r="P23" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="2" t="s">
+      <c r="J23" s="2">
+        <v>1</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1</v>
+      </c>
+      <c r="L23" s="10"/>
+      <c r="O23" s="2">
+        <v>1</v>
+      </c>
+      <c r="P23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="R23"/>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>2</v>
       </c>
@@ -2129,52 +2122,52 @@
       <c r="G24" s="2">
         <v>20</v>
       </c>
-      <c r="H24" s="2">
-        <v>6</v>
-      </c>
-      <c r="I24" s="2"/>
-      <c r="J24" s="7">
+      <c r="H24" s="7">
         <v>30000</v>
       </c>
-      <c r="K24" s="7">
+      <c r="I24" s="7">
         <v>180000</v>
       </c>
-      <c r="L24" s="2">
-        <v>1</v>
-      </c>
-      <c r="M24" s="2">
+      <c r="J24" s="2">
+        <v>1</v>
+      </c>
+      <c r="K24" s="2">
         <v>2</v>
       </c>
-      <c r="N24" s="10"/>
-      <c r="P24" s="2">
+      <c r="L24" s="10"/>
+      <c r="O24" s="2">
         <v>2</v>
       </c>
-      <c r="Q24" s="2" t="s">
+      <c r="P24" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="R24"/>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
       <c r="P25"/>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B29" s="55" t="s">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B29" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="55"/>
-      <c r="L29" s="55"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="42"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="43"/>
+      <c r="K29"/>
+      <c r="L29"/>
       <c r="N29"/>
-      <c r="O29"/>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="O29" s="65" t="s">
+        <v>106</v>
+      </c>
+      <c r="P29" s="66"/>
+      <c r="Q29" s="66"/>
+      <c r="R29" s="67"/>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>29</v>
       </c>
@@ -2191,35 +2184,34 @@
         <v>21</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="H30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="O30" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="J30" s="2" t="s">
+      <c r="P30" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q30" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="R30" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="L30" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="M30"/>
-      <c r="N30"/>
-      <c r="P30" s="58" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q30" s="58"/>
-      <c r="R30" s="58"/>
-      <c r="S30" s="58"/>
-      <c r="T30" s="58"/>
-      <c r="U30" s="58"/>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="S30"/>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B31" s="2">
         <v>1</v>
       </c>
@@ -2238,43 +2230,31 @@
       <c r="G31" s="2">
         <v>20</v>
       </c>
-      <c r="H31" s="2">
-        <v>5</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="J31" s="7">
+      <c r="H31" s="7">
         <v>30000</v>
       </c>
-      <c r="K31" s="7">
+      <c r="I31" s="7">
         <v>150000</v>
       </c>
-      <c r="L31" s="2">
-        <v>1</v>
-      </c>
-      <c r="M31"/>
-      <c r="N31"/>
+      <c r="J31" s="2">
+        <v>1</v>
+      </c>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="O31" s="2">
+        <v>1</v>
+      </c>
       <c r="P31" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R31" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="S31" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="T31" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="U31" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="Q31" s="7">
+        <v>20000</v>
+      </c>
+      <c r="R31" s="7">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B32" s="2">
         <v>2</v>
       </c>
@@ -2294,78 +2274,48 @@
         <v>25</v>
       </c>
       <c r="H32" s="2">
-        <v>6</v>
-      </c>
-      <c r="I32" s="2"/>
+        <v>40000</v>
+      </c>
+      <c r="I32" s="7">
+        <v>240000</v>
+      </c>
       <c r="J32" s="2">
-        <v>40000</v>
-      </c>
-      <c r="K32" s="7">
-        <v>240000</v>
-      </c>
-      <c r="L32" s="2">
         <v>2</v>
       </c>
-      <c r="M32"/>
-      <c r="N32"/>
-      <c r="P32" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q32" s="2" t="s">
-        <v>106</v>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="O32" s="2">
+        <v>2</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q32" s="7">
+        <v>25000</v>
       </c>
       <c r="R32" s="7">
-        <v>20000</v>
-      </c>
-      <c r="S32" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="T32" s="2">
-        <v>20</v>
-      </c>
-      <c r="U32" s="7">
-        <v>400000</v>
-      </c>
-    </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="P33" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q33" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="R33" s="7">
-        <v>25000</v>
-      </c>
-      <c r="S33" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="T33" s="2">
-        <v>10</v>
-      </c>
-      <c r="U33" s="7">
         <v>250000</v>
       </c>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B38" s="56" t="s">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B38" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="56"/>
-      <c r="F38" s="56"/>
-      <c r="G38" s="56"/>
-      <c r="H38" s="56"/>
-      <c r="I38" s="56"/>
-      <c r="J38" s="56"/>
-      <c r="K38" s="56"/>
-      <c r="L38" s="56"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="50"/>
+      <c r="E38" s="50"/>
+      <c r="F38" s="50"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
+      <c r="I38" s="50"/>
+      <c r="J38" s="51"/>
+      <c r="K38"/>
+      <c r="L38"/>
       <c r="N38"/>
       <c r="O38"/>
       <c r="P38"/>
     </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B39" s="2" t="s">
         <v>35</v>
       </c>
@@ -2382,31 +2332,25 @@
         <v>21</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K39" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="L39" s="17" t="s">
+      <c r="J39" s="17" t="s">
         <v>41</v>
       </c>
+      <c r="K39"/>
+      <c r="L39"/>
       <c r="M39"/>
       <c r="N39"/>
       <c r="O39"/>
       <c r="P39"/>
-      <c r="Q39"/>
-      <c r="R39"/>
-    </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B40" s="2">
         <v>1</v>
       </c>
@@ -2425,27 +2369,21 @@
       <c r="G40" s="2">
         <v>4</v>
       </c>
-      <c r="H40" s="2">
-        <v>5</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="J40" s="7">
+      <c r="H40" s="7">
         <v>40000</v>
       </c>
-      <c r="K40" s="7">
+      <c r="I40" s="7">
         <v>160000</v>
       </c>
-      <c r="L40" s="2">
-        <v>1</v>
-      </c>
-      <c r="M40"/>
+      <c r="J40" s="2">
+        <v>1</v>
+      </c>
+      <c r="K40"/>
+      <c r="N40"/>
+      <c r="O40"/>
       <c r="P40"/>
-      <c r="Q40"/>
-      <c r="R40"/>
-    </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B41" s="2">
         <v>2</v>
       </c>
@@ -2464,54 +2402,50 @@
       <c r="G41" s="2">
         <v>3</v>
       </c>
-      <c r="H41" s="2">
-        <v>6</v>
-      </c>
-      <c r="I41" s="2"/>
-      <c r="J41" s="7">
+      <c r="H41" s="7">
         <v>10000</v>
       </c>
-      <c r="K41" s="7">
+      <c r="I41" s="7">
         <v>30000</v>
       </c>
-      <c r="L41" s="2">
+      <c r="J41" s="2">
         <v>2</v>
       </c>
-      <c r="M41"/>
-      <c r="P41"/>
-      <c r="Q41"/>
-    </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="K41"/>
+      <c r="N41"/>
+      <c r="O41"/>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.2">
       <c r="P44"/>
     </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.2">
       <c r="P45"/>
     </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.2">
       <c r="N46"/>
       <c r="O46"/>
       <c r="P46"/>
     </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B47" s="31" t="s">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B47" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="C47" s="31"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31"/>
-      <c r="H47" s="31"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
-      <c r="K47" s="31"/>
-      <c r="L47" s="31"/>
-      <c r="M47" s="31"/>
+      <c r="C47" s="61"/>
+      <c r="D47" s="61"/>
+      <c r="E47" s="61"/>
+      <c r="F47" s="61"/>
+      <c r="G47" s="61"/>
+      <c r="H47" s="61"/>
+      <c r="I47" s="61"/>
+      <c r="J47" s="62"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
       <c r="N47"/>
       <c r="O47"/>
       <c r="P47"/>
     </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
         <v>37</v>
       </c>
@@ -2521,40 +2455,31 @@
       <c r="D48" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E48" s="22" t="s">
-        <v>38</v>
+      <c r="E48" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>95</v>
+        <v>39</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>39</v>
+        <v>105</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I48" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="J48" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="K48" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="L48" s="2" t="s">
+      <c r="I48" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="M48" s="17" t="s">
+      <c r="J48" s="17" t="s">
         <v>41</v>
       </c>
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
       <c r="N48"/>
       <c r="O48"/>
-      <c r="P48"/>
-      <c r="Q48"/>
-      <c r="R48"/>
-    </row>
-    <row r="49" spans="2:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B49" s="2">
         <v>1</v>
       </c>
@@ -2564,40 +2489,31 @@
       <c r="D49" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E49" s="22" t="s">
+      <c r="E49" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F49" s="2" t="s">
-        <v>72</v>
+      <c r="F49" s="2">
+        <v>2</v>
       </c>
       <c r="G49" s="2">
-        <v>2</v>
-      </c>
-      <c r="H49" s="2">
         <v>4</v>
       </c>
-      <c r="I49" s="22">
-        <v>5</v>
-      </c>
-      <c r="J49" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="K49" s="7">
+      <c r="H49" s="7">
         <v>45000</v>
       </c>
-      <c r="L49" s="7">
+      <c r="I49" s="7">
         <v>180000</v>
       </c>
-      <c r="M49" s="2">
-        <v>1</v>
-      </c>
+      <c r="J49" s="2">
+        <v>1</v>
+      </c>
+      <c r="K49"/>
+      <c r="L49"/>
+      <c r="M49"/>
       <c r="N49"/>
       <c r="O49"/>
-      <c r="P49"/>
-      <c r="Q49"/>
-      <c r="R49"/>
-    </row>
-    <row r="50" spans="2:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B50" s="2">
         <v>2</v>
       </c>
@@ -2607,45 +2523,38 @@
       <c r="D50" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E50" s="22">
-        <v>8</v>
-      </c>
-      <c r="F50" s="2">
+      <c r="E50" s="2">
         <v>20</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="H50" s="2">
+      <c r="G50" s="2">
         <v>6</v>
       </c>
-      <c r="I50" s="22">
-        <v>6</v>
-      </c>
-      <c r="J50" s="22"/>
-      <c r="K50" s="7">
+      <c r="H50" s="7">
         <v>30000</v>
       </c>
-      <c r="L50" s="7">
+      <c r="I50" s="7">
         <v>180000</v>
       </c>
-      <c r="M50" s="2">
+      <c r="J50" s="2">
         <v>2</v>
       </c>
-      <c r="N50"/>
-      <c r="O50"/>
-    </row>
-    <row r="56" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B56" s="59" t="s">
+      <c r="K50"/>
+      <c r="L50"/>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B56" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="C56" s="60"/>
-      <c r="D56" s="60"/>
-      <c r="E56" s="61"/>
+      <c r="C56" s="54"/>
+      <c r="D56" s="54"/>
+      <c r="E56" s="55"/>
       <c r="F56"/>
       <c r="G56"/>
     </row>
-    <row r="57" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="s">
         <v>41</v>
       </c>
@@ -2659,7 +2568,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="58" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B58" s="2">
         <v>1</v>
       </c>
@@ -2667,13 +2576,13 @@
         <v>77</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B59" s="2">
         <v>2</v>
       </c>
@@ -2681,184 +2590,196 @@
         <v>86</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E59" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B60"/>
       <c r="C60"/>
       <c r="D60"/>
     </row>
-    <row r="61" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B61"/>
       <c r="C61"/>
       <c r="D61"/>
     </row>
-    <row r="62" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B62"/>
       <c r="C62"/>
       <c r="D62"/>
     </row>
-    <row r="63" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B63"/>
       <c r="C63"/>
       <c r="D63"/>
     </row>
-    <row r="64" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B64"/>
       <c r="C64"/>
       <c r="D64"/>
     </row>
-    <row r="65" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B65"/>
-      <c r="C65"/>
-      <c r="D65"/>
-    </row>
-    <row r="66" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B66"/>
-      <c r="C66"/>
-      <c r="D66"/>
-    </row>
-    <row r="67" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B67" s="47" t="s">
+    <row r="65" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B65" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="C67" s="47"/>
-      <c r="D67" s="47"/>
-      <c r="E67" s="47"/>
-      <c r="F67" s="47"/>
-      <c r="G67" s="47"/>
-      <c r="H67" s="47"/>
-      <c r="I67" s="47"/>
-      <c r="J67" s="47"/>
-      <c r="K67" s="47"/>
-      <c r="L67" s="47"/>
-      <c r="M67"/>
-    </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B68" s="2" t="s">
+      <c r="C65" s="64"/>
+      <c r="D65" s="64"/>
+      <c r="E65" s="64"/>
+      <c r="F65" s="64"/>
+      <c r="G65" s="64"/>
+      <c r="H65" s="64"/>
+      <c r="I65" s="64"/>
+      <c r="J65" s="64"/>
+      <c r="K65" s="64"/>
+      <c r="L65" s="64"/>
+      <c r="M65" s="64"/>
+    </row>
+    <row r="66" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B66" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C68" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D68" s="12" t="s">
+      <c r="C66" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G66" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="H66" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E68" s="13" t="s">
+      <c r="I66" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F68" s="14" t="s">
+      <c r="J66" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="G68" s="15" t="s">
+      <c r="K66" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="H68" s="20" t="s">
+      <c r="L66" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="I68" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="J68" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="K68" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L68" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B69" s="2">
-        <v>1</v>
-      </c>
-      <c r="C69" s="2">
-        <v>1</v>
-      </c>
-      <c r="D69" s="2">
-        <v>1</v>
-      </c>
-      <c r="E69" s="2">
+      <c r="M66" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="N66"/>
+      <c r="O66"/>
+      <c r="P66"/>
+    </row>
+    <row r="67" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B67" s="2">
+        <v>1</v>
+      </c>
+      <c r="C67" s="5">
+        <v>45209</v>
+      </c>
+      <c r="D67" s="5">
+        <v>45211</v>
+      </c>
+      <c r="E67" s="2">
+        <v>23</v>
+      </c>
+      <c r="F67" s="2">
+        <v>350000</v>
+      </c>
+      <c r="G67" s="2">
+        <v>1</v>
+      </c>
+      <c r="H67" s="2">
+        <v>1</v>
+      </c>
+      <c r="I67" s="2">
         <v>2</v>
       </c>
-      <c r="F69" s="2">
+      <c r="J67" s="2">
         <v>3</v>
       </c>
-      <c r="G69" s="2">
-        <v>1</v>
-      </c>
-      <c r="H69" s="2">
-        <v>1</v>
-      </c>
-      <c r="I69" s="2">
+      <c r="K67" s="2">
+        <v>1</v>
+      </c>
+      <c r="L67" s="2">
+        <v>1</v>
+      </c>
+      <c r="M67" s="2">
         <v>2</v>
       </c>
-      <c r="J69" s="5">
-        <v>45209</v>
-      </c>
-      <c r="K69" s="2">
-        <v>23</v>
-      </c>
-      <c r="L69" s="2">
-        <v>350000</v>
-      </c>
-    </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="N67"/>
+      <c r="O67"/>
+      <c r="P67"/>
+    </row>
+    <row r="68" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B68"/>
+      <c r="C68"/>
+      <c r="D68"/>
+    </row>
+    <row r="69" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B69"/>
+      <c r="C69"/>
+      <c r="D69"/>
+    </row>
+    <row r="70" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B70"/>
       <c r="C70"/>
       <c r="D70"/>
     </row>
-    <row r="71" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B71"/>
       <c r="C71"/>
       <c r="D71"/>
     </row>
-    <row r="72" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B72"/>
       <c r="C72"/>
       <c r="D72"/>
     </row>
-    <row r="73" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B73"/>
       <c r="C73"/>
       <c r="D73"/>
     </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B74"/>
       <c r="C74"/>
       <c r="D74"/>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B75"/>
       <c r="C75"/>
       <c r="D75"/>
     </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B76"/>
       <c r="C76"/>
       <c r="D76"/>
     </row>
-    <row r="77" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B77"/>
       <c r="C77"/>
       <c r="D77"/>
     </row>
-    <row r="78" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B78"/>
       <c r="C78"/>
       <c r="D78"/>
     </row>
-    <row r="79" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B79"/>
       <c r="C79"/>
       <c r="D79"/>
     </row>
-    <row r="80" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B80"/>
       <c r="C80"/>
       <c r="D80"/>
@@ -2878,29 +2799,16 @@
       <c r="C83"/>
       <c r="D83"/>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B84"/>
-      <c r="C84"/>
-      <c r="D84"/>
-    </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B85"/>
-      <c r="C85"/>
-      <c r="D85"/>
-    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="8">
+    <mergeCell ref="B21:K21"/>
+    <mergeCell ref="B29:J29"/>
+    <mergeCell ref="B38:J38"/>
     <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B47:M47"/>
     <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B67:L67"/>
     <mergeCell ref="B12:F12"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="B21:M21"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="P30:U30"/>
+    <mergeCell ref="B47:J47"/>
+    <mergeCell ref="B65:M65"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G5" r:id="rId1" xr:uid="{75F1E996-0DAC-A046-8A72-3230C587CEA0}"/>

</xml_diff>